<commit_message>
Sales Report and Excel added || Reduced latency in responses
</commit_message>
<xml_diff>
--- a/sales_report.xlsx
+++ b/sales_report.xlsx
@@ -348,7 +348,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>68</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3">
@@ -356,7 +356,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>348123.73</v>
+        <v>117940</v>
       </c>
     </row>
     <row r="4">
@@ -364,7 +364,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>1860</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5">
@@ -372,7 +372,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>1860</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Invoice and Wallet Transactions History implemented
</commit_message>
<xml_diff>
--- a/sales_report.xlsx
+++ b/sales_report.xlsx
@@ -348,7 +348,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>7</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3">
@@ -356,7 +356,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>117940</v>
+        <v>417640</v>
       </c>
     </row>
     <row r="4">
@@ -364,7 +364,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>60</v>
+        <v>4760</v>
       </c>
     </row>
     <row r="5">
@@ -372,7 +372,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>60</v>
+        <v>4760</v>
       </c>
     </row>
   </sheetData>

</xml_diff>